<commit_message>
feat - add scenario where correlated features are removed before feature selection
</commit_message>
<xml_diff>
--- a/final_project/results/metrics.xlsx
+++ b/final_project/results/metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,62 +466,87 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>mse_4</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>mae_1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>mae_2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>mae_3</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>mae_4</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>r2_1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>r2_2</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>r2_3</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>r2_4</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>rmse_1</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>rmse_2</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>rmse_3</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_4</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>explained_variance_score_1</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>explained_variance_score_2</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>explained_variance_score_3</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>explained_variance_score_4</t>
         </is>
       </c>
     </row>
@@ -538,53 +563,68 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'max_depth': 3, 'max_features': 'sqrt', 'n_estimators': 100}</t>
+          <t>{'max_depth': 5, 'max_features': 'sqrt', 'n_estimators': 200}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>48.96379521773041</v>
+        <v>40.04541689428554</v>
       </c>
       <c r="E2" t="n">
-        <v>244.1517976581676</v>
+        <v>214.6325086822381</v>
       </c>
       <c r="F2" t="n">
-        <v>83.38784542854424</v>
+        <v>119.8564870303817</v>
       </c>
       <c r="G2" t="n">
-        <v>5.784872154500943</v>
+        <v>8.793242478804412</v>
       </c>
       <c r="H2" t="n">
-        <v>12.47088027363486</v>
+        <v>5.136627284613351</v>
       </c>
       <c r="I2" t="n">
-        <v>5.417529556378404</v>
+        <v>11.42074789772591</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4831291052877383</v>
+        <v>6.414199043720438</v>
       </c>
       <c r="K2" t="n">
-        <v>0.483976082066722</v>
+        <v>2.270428510133486</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5862483926374839</v>
+        <v>0.4502982455585148</v>
       </c>
       <c r="M2" t="n">
-        <v>6.997413466255257</v>
+        <v>0.5557785214373216</v>
       </c>
       <c r="N2" t="n">
-        <v>15.62535752097108</v>
+        <v>0.3854610372806777</v>
       </c>
       <c r="O2" t="n">
-        <v>9.13169455405426</v>
+        <v>0.7620564316620487</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4831592403315896</v>
+        <v>6.328144822480404</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.497362613240156</v>
+        <v>14.65034158926808</v>
       </c>
       <c r="R2" t="n">
-        <v>0.6041925912263503</v>
+        <v>10.94789874954923</v>
+      </c>
+      <c r="S2" t="n">
+        <v>2.96534019613339</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.4504620211856515</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.5593789900154709</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.398797216794625</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.7632133834531998</v>
       </c>
     </row>
     <row r="3">
@@ -600,53 +640,68 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'max_depth': 3, 'max_features': 'sqrt', 'n_estimators': 100}</t>
+          <t>{'max_depth': 5, 'max_features': 'sqrt', 'n_estimators': 200}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>52.54749440231157</v>
+        <v>40.14218905947948</v>
       </c>
       <c r="E3" t="n">
-        <v>235.9239859731668</v>
+        <v>213.4599595244804</v>
       </c>
       <c r="F3" t="n">
-        <v>100.8117139685479</v>
+        <v>125.5264908354093</v>
       </c>
       <c r="G3" t="n">
-        <v>5.841386811520666</v>
+        <v>8.940881991106414</v>
       </c>
       <c r="H3" t="n">
-        <v>12.10554885381961</v>
+        <v>5.116789038759141</v>
       </c>
       <c r="I3" t="n">
-        <v>5.30689224989563</v>
+        <v>11.19745738608311</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4452989126795616</v>
+        <v>6.541019558356266</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5013658685128399</v>
+        <v>2.222201615572862</v>
       </c>
       <c r="L3" t="n">
-        <v>0.4997951022586445</v>
+        <v>0.4489698581146124</v>
       </c>
       <c r="M3" t="n">
-        <v>7.248965057324499</v>
+        <v>0.5582053277200442</v>
       </c>
       <c r="N3" t="n">
-        <v>15.35981725064354</v>
+        <v>0.3563892836919627</v>
       </c>
       <c r="O3" t="n">
-        <v>10.04050367105893</v>
+        <v>0.7580613328723257</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4454362478231882</v>
+        <v>6.335786380511852</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5098540877356471</v>
+        <v>14.6102689750901</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5144933429868529</v>
+        <v>11.20386053266504</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2.990130764884107</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.4492700227126445</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.5616106088729953</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.3717605509266285</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.7599249758949355</v>
       </c>
     </row>
     <row r="4">
@@ -662,53 +717,68 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'max_depth': 3, 'max_features': 'sqrt', 'n_estimators': 100}</t>
+          <t>{'max_depth': 5, 'max_features': 'sqrt', 'n_estimators': 200}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>54.22621189472168</v>
+        <v>41.17807625865857</v>
       </c>
       <c r="E4" t="n">
-        <v>222.3180494896138</v>
+        <v>203.7438493446589</v>
       </c>
       <c r="F4" t="n">
-        <v>87.0455598738838</v>
+        <v>126.7072263582291</v>
       </c>
       <c r="G4" t="n">
-        <v>5.97706169474442</v>
+        <v>9.074364885284091</v>
       </c>
       <c r="H4" t="n">
-        <v>11.85320562784704</v>
+        <v>5.189926296555458</v>
       </c>
       <c r="I4" t="n">
-        <v>5.198190855587611</v>
+        <v>11.07045318071319</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4275780597838094</v>
+        <v>6.588301788985013</v>
       </c>
       <c r="K4" t="n">
-        <v>0.530122522032239</v>
+        <v>2.263723825469939</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5680996417823108</v>
+        <v>0.4347502780738941</v>
       </c>
       <c r="M4" t="n">
-        <v>7.363844912457193</v>
+        <v>0.5783146059298432</v>
       </c>
       <c r="N4" t="n">
-        <v>14.91033364783008</v>
+        <v>0.3503353102991367</v>
       </c>
       <c r="O4" t="n">
-        <v>9.329820999026927</v>
+        <v>0.7544493096363837</v>
       </c>
       <c r="P4" t="n">
-        <v>0.4275790100712931</v>
+        <v>6.417014590809232</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.5403745423005701</v>
+        <v>14.27388697393457</v>
       </c>
       <c r="R4" t="n">
-        <v>0.5835167812705242</v>
+        <v>11.25643044478262</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3.012368650295659</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.4348767080115156</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.5840649168823479</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.3677891057809866</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.7568776181649078</v>
       </c>
     </row>
     <row r="5">
@@ -724,53 +794,376 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'max_depth': 3, 'max_features': 'sqrt', 'n_estimators': 100}</t>
+          <t>{'max_depth': 5, 'max_features': 'sqrt', 'n_estimators': 200}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>53.08413946636868</v>
+        <v>40.67302149982101</v>
       </c>
       <c r="E5" t="n">
-        <v>254.1790694283168</v>
+        <v>209.0643741551446</v>
       </c>
       <c r="F5" t="n">
-        <v>89.82758245919358</v>
+        <v>126.0678816918444</v>
       </c>
       <c r="G5" t="n">
-        <v>5.964665028903434</v>
+        <v>9.491560969275879</v>
       </c>
       <c r="H5" t="n">
-        <v>12.71424322118714</v>
+        <v>5.106866505615931</v>
       </c>
       <c r="I5" t="n">
-        <v>5.744063013897397</v>
+        <v>11.19928891612536</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4396339879495913</v>
+        <v>6.643890935514915</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4627830697086538</v>
+        <v>2.3379739349392</v>
       </c>
       <c r="L5" t="n">
-        <v>0.5542958756521845</v>
+        <v>0.4416831435190194</v>
       </c>
       <c r="M5" t="n">
-        <v>7.285886319890579</v>
+        <v>0.5673028006233948</v>
       </c>
       <c r="N5" t="n">
-        <v>15.94299436832105</v>
+        <v>0.3536134157887506</v>
       </c>
       <c r="O5" t="n">
-        <v>9.477741421836406</v>
+        <v>0.7431600582412461</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4400310337669051</v>
+        <v>6.377540395781199</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4732730386104265</v>
+        <v>14.4590585500974</v>
       </c>
       <c r="R5" t="n">
-        <v>0.572349389674643</v>
+        <v>11.22799544406055</v>
+      </c>
+      <c r="S5" t="n">
+        <v>3.080837705767034</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.4418635536516377</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.5730165550813762</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.3709540123000195</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.7453670890052116</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>rfe_corr</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'max_depth': 5, 'max_features': 'sqrt', 'n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>40.05655414927478</v>
+      </c>
+      <c r="E6" t="n">
+        <v>203.47848701386</v>
+      </c>
+      <c r="F6" t="n">
+        <v>123.5383768435975</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9.771522327320266</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5.094473333020188</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10.95964807388055</v>
+      </c>
+      <c r="J6" t="n">
+        <v>6.518491389504591</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2.356047213162978</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.4501453649274202</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5788638221118001</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.366582920603631</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.7355843539785248</v>
+      </c>
+      <c r="P6" t="n">
+        <v>6.329024739189663</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>14.26458856798401</v>
+      </c>
+      <c r="R6" t="n">
+        <v>11.11478190715398</v>
+      </c>
+      <c r="S6" t="n">
+        <v>3.125943429961628</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.4502747978767251</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.5824824333028951</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.3826327080480995</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.7373689439010525</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mutual information_corr</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'max_depth': 5, 'max_features': 'sqrt', 'n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>40.2268175853126</v>
+      </c>
+      <c r="E7" t="n">
+        <v>200.7873083473967</v>
+      </c>
+      <c r="F7" t="n">
+        <v>125.6237779757079</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8.681919101944013</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5.09887530177093</v>
+      </c>
+      <c r="I7" t="n">
+        <v>10.76096389933431</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6.451401761038793</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2.228435533249391</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.4478081658977708</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.5844337116575751</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.3558904643141689</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.7650688223237919</v>
+      </c>
+      <c r="P7" t="n">
+        <v>6.342461476848921</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>14.16994383712923</v>
+      </c>
+      <c r="R7" t="n">
+        <v>11.20820137112587</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2.946509647352951</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.4481598540843266</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.5868783505891328</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.3709231820556166</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.7663632148446653</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>random forest_corr</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>{'max_depth': 5, 'max_features': 'log2', 'n_estimators': 100}</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>40.70295956872089</v>
+      </c>
+      <c r="E8" t="n">
+        <v>194.5403292514916</v>
+      </c>
+      <c r="F8" t="n">
+        <v>120.2025904088349</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9.12013497668109</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5.133752998733526</v>
+      </c>
+      <c r="I8" t="n">
+        <v>10.84182255368582</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6.300779495866182</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2.311065422163566</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.4412721849056456</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.597362984616135</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.383686464902844</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.753210779151593</v>
+      </c>
+      <c r="P8" t="n">
+        <v>6.379887112537406</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>13.94777147975588</v>
+      </c>
+      <c r="R8" t="n">
+        <v>10.96369419533557</v>
+      </c>
+      <c r="S8" t="n">
+        <v>3.019956121648308</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.4415351882678781</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.6027332514360879</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.398366720820723</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.7558258233020325</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>all_corr</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>{'max_depth': 5, 'max_features': 'sqrt', 'n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>40.12007187002515</v>
+      </c>
+      <c r="E9" t="n">
+        <v>211.3727720449667</v>
+      </c>
+      <c r="F9" t="n">
+        <v>125.116086554535</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9.866569880249202</v>
+      </c>
+      <c r="H9" t="n">
+        <v>5.083135340004559</v>
+      </c>
+      <c r="I9" t="n">
+        <v>11.41540945082701</v>
+      </c>
+      <c r="J9" t="n">
+        <v>6.579528485003495</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.391660088193357</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.4492734598445794</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.5625251463434184</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.3584935454412672</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.7330123842005715</v>
+      </c>
+      <c r="P9" t="n">
+        <v>6.334040722163471</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>14.53866472702933</v>
+      </c>
+      <c r="R9" t="n">
+        <v>11.18553023126463</v>
+      </c>
+      <c r="S9" t="n">
+        <v>3.141109657469666</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.4493366191766381</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.5668259992564464</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.3732732254189337</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.7351386177576507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>